<commit_message>
Removed About Page, Fixes To Upload Excel File Function
</commit_message>
<xml_diff>
--- a/static/uploads/excels/ratings.xlsx
+++ b/static/uploads/excels/ratings.xlsx
@@ -3,17 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26812"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8FD7DC1D-81E3-4113-9050-8A266E390D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5A25A65-1142-4BC4-A6ED-CDAAF8483024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -330,32 +326,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Calc"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Tables"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -657,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:P1"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="P125" sqref="P125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>